<commit_message>
Includes Institution’s Upper Limit of Days for EXP
</commit_message>
<xml_diff>
--- a/Expense Report Review Calculator.xlsx
+++ b/Expense Report Review Calculator.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Personal Vault\Careers\Useful Job Tools\EXP Calculators\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hihipy\coding-workspace\useful-job-tools\Expense-Report-Review-Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6774ED-B0A6-463A-88E0-5F2B21AD4AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D324471-6221-4555-9714-432211272911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9EB0749C-90DE-4314-8D7D-2707C09E549F}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Page #</t>
   </si>
@@ -84,9 +84,6 @@
     <t># of Expenses:</t>
   </si>
   <si>
-    <t>60 Days Ago Date</t>
-  </si>
-  <si>
     <t>USER INPUT REQUIRED</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>OPTIONAL FIELD</t>
+  </si>
+  <si>
+    <t>Institution’s Upper Limit of Days After Expense was Paid or Incurred</t>
   </si>
 </sst>
 </file>
@@ -103,8 +103,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="[$USD]\ #,##0.00"/>
-    <numFmt numFmtId="168" formatCode="_([$USD]\ * #,##0.00_);_([$USD]\ * \(#,##0.00\);_([$USD]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="[$USD]\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="_([$USD]\ * #,##0.00_);_([$USD]\ * \(#,##0.00\);_([$USD]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -307,11 +307,8 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -334,9 +331,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -363,12 +357,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -378,10 +378,19 @@
     <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -405,7 +414,7 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="168" formatCode="_([$USD]\ * #,##0.00_);_([$USD]\ * \(#,##0.00\);_([$USD]\ * &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -437,7 +446,7 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <numFmt numFmtId="166" formatCode="_([$USD]\ * #,##0.00_);_([$USD]\ * \(#,##0.00\);_([$USD]\ * &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -453,7 +462,7 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -528,15 +537,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8C5EBB0-BFD2-43B5-9865-41A9B951F4B6}" name="Table1" displayName="Table1" ref="A7:E54" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A7:E54" xr:uid="{FC060CE5-3EF0-4040-92D1-4AED472000A2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8C5EBB0-BFD2-43B5-9865-41A9B951F4B6}" name="Table1" displayName="Table1" ref="A8:E55" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A8:E55" xr:uid="{FC060CE5-3EF0-4040-92D1-4AED472000A2}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{931DCCE9-E379-43B2-91F7-D4E1BD90235B}" name="Page #" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{847CC89E-9549-4D2E-A289-5BA063AB0767}" name="Date of Expense" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{F7577957-29D5-4CA4-BB08-E2352CA02DC2}" name="USD" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{847CC89E-9549-4D2E-A289-5BA063AB0767}" name="Date of Expense" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{F7577957-29D5-4CA4-BB08-E2352CA02DC2}" name="USD" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{86E9BD60-88D4-4DBA-8863-1E4B3672BE98}" name="Notes" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{94442348-A842-4B9E-8438-186F22B4E931}" name="# Days &gt;60" dataDxfId="3">
-      <calculatedColumnFormula array="1">_xlfn.IFS(OR(ISERROR(B$2-B8), ISBLANK(B8), ISBLANK(C8)), "Enter Data in both Row 1 &amp; Starting at Row 8", B$2&gt;B8, B$2-B8, TRUE, "N/A")</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{94442348-A842-4B9E-8438-186F22B4E931}" name="# Days &gt;60" dataDxfId="0">
+      <calculatedColumnFormula array="1">_xlfn.IFS(OR(ISERROR(B$3-B9), ISBLANK(B9), ISBLANK(C9)), "Enter Data in both Row 1 &amp; Starting at Row 8", B$3&gt;B9, B$3-B9, TRUE, "N/A")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -841,619 +850,631 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5382BE5-3DC5-4059-BA39-DC147037E46F}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="58.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="58.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="str">
+        <f>B2&amp;" Days Ago Date"</f>
+        <v xml:space="preserve"> Days Ago Date</v>
+      </c>
+      <c r="B3" s="22" t="str">
+        <f>IF(ISBLANK(B1), "Enter EXP Submission Date at Row 1", B1-B2)</f>
+        <v>Enter EXP Submission Date at Row 1</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="20" t="str">
+        <f>IF(OR(ISBLANK(B9), ISBLANK(C9), ISBLANK(B1)),"Enter Data Starting in Rows 1 &amp; 8", SUM(Table1[USD]))</f>
+        <v>Enter Data Starting in Rows 1 &amp; 8</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="18" t="str">
+        <f>IF(OR(ISBLANK(B9), ISBLANK(C9), ISBLANK(B1)),"Enter Data Starting in Rows 1 &amp; 8", COUNTA(Table1[Date of Expense]))</f>
+        <v>Enter Data Starting in Rows 1 &amp; 8</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="22" t="str">
-        <f>IF(ISBLANK(B1), "Enter EXP Submission Date at Row 1", B1-60)</f>
-        <v>Enter EXP Submission Date at Row 1</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="7" t="s">
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="24" t="str">
-        <f>IF(OR(ISBLANK(B8), ISBLANK(C8), ISBLANK(B1)),"Enter Data Starting in Rows 1 &amp; 8", SUM(Table1[USD]))</f>
+      <c r="E7" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="15" t="str" cm="1">
+        <f t="array" ref="E9">_xlfn.IFS(OR(ISERROR(B$3-B9), ISBLANK(B9), ISBLANK(C9)), "Enter Data Starting in Rows 1 &amp; 8", B$3&gt;B9, B$3-B9, TRUE, "N/A")</f>
         <v>Enter Data Starting in Rows 1 &amp; 8</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="19" t="str">
-        <f>IF(OR(ISBLANK(B8), ISBLANK(C8), ISBLANK(B1)),"Enter Data Starting in Rows 1 &amp; 8", COUNTA(Table1[Date of Expense]))</f>
-        <v>Enter Data Starting in Rows 1 &amp; 8</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="17" t="str" cm="1">
-        <f t="array" ref="E8">_xlfn.IFS(OR(ISERROR(B$2-B8), ISBLANK(B8), ISBLANK(C8)), "Enter Data Starting in Rows 1 &amp; 8", B$2&gt;B8, B$2-B8, TRUE, "N/A")</f>
-        <v>Enter Data Starting in Rows 1 &amp; 8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="17" t="str" cm="1">
-        <f t="array" ref="E9">_xlfn.IFS(OR(ISBLANK(B9), ISBLANK(C9)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B9, B$2-B9, TRUE, "N/A")</f>
-        <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
-      </c>
-      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="17" t="str" cm="1">
-        <f t="array" ref="E10">_xlfn.IFS(OR(ISBLANK(B10), ISBLANK(C10)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B10, B$2-B10, TRUE, "N/A")</f>
-        <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
-      </c>
+      <c r="A10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="15" t="str" cm="1">
+        <f t="array" ref="E10">_xlfn.IFS(OR(ISBLANK(B10), ISBLANK(C10)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B10, B$3-B10, TRUE, "N/A")</f>
+        <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
+      </c>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="17" t="str" cm="1">
-        <f t="array" ref="E11">_xlfn.IFS(OR(ISBLANK(B11), ISBLANK(C11)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B11, B$2-B11, TRUE, "N/A")</f>
+      <c r="A11" s="11"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="15" t="str" cm="1">
+        <f t="array" ref="E11">_xlfn.IFS(OR(ISBLANK(B11), ISBLANK(C11)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B11, B$3-B11, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="17" t="str" cm="1">
-        <f t="array" ref="E12">_xlfn.IFS(OR(ISBLANK(B12), ISBLANK(C12)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B12, B$2-B12, TRUE, "N/A")</f>
+      <c r="A12" s="11"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="15" t="str" cm="1">
+        <f t="array" ref="E12">_xlfn.IFS(OR(ISBLANK(B12), ISBLANK(C12)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B12, B$3-B12, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="17" t="str" cm="1">
-        <f t="array" ref="E13">_xlfn.IFS(OR(ISBLANK(B13), ISBLANK(C13)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B13, B$2-B13, TRUE, "N/A")</f>
+      <c r="A13" s="11"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="15" t="str" cm="1">
+        <f t="array" ref="E13">_xlfn.IFS(OR(ISBLANK(B13), ISBLANK(C13)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B13, B$3-B13, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="17" t="str" cm="1">
-        <f t="array" ref="E14">_xlfn.IFS(OR(ISBLANK(B14), ISBLANK(C14)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B14, B$2-B14, TRUE, "N/A")</f>
+      <c r="A14" s="11"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="15" t="str" cm="1">
+        <f t="array" ref="E14">_xlfn.IFS(OR(ISBLANK(B14), ISBLANK(C14)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B14, B$3-B14, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="17" t="str" cm="1">
-        <f t="array" ref="E15">_xlfn.IFS(OR(ISBLANK(B15), ISBLANK(C15)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B15, B$2-B15, TRUE, "N/A")</f>
+      <c r="A15" s="11"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="15" t="str" cm="1">
+        <f t="array" ref="E15">_xlfn.IFS(OR(ISBLANK(B15), ISBLANK(C15)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B15, B$3-B15, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="17" t="str" cm="1">
-        <f t="array" ref="E16">_xlfn.IFS(OR(ISBLANK(B16), ISBLANK(C16)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B16, B$2-B16, TRUE, "N/A")</f>
+      <c r="A16" s="11"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="15" t="str" cm="1">
+        <f t="array" ref="E16">_xlfn.IFS(OR(ISBLANK(B16), ISBLANK(C16)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B16, B$3-B16, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="17" t="str" cm="1">
-        <f t="array" ref="E17">_xlfn.IFS(OR(ISBLANK(B17), ISBLANK(C17)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B17, B$2-B17, TRUE, "N/A")</f>
+      <c r="A17" s="11"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="15" t="str" cm="1">
+        <f t="array" ref="E17">_xlfn.IFS(OR(ISBLANK(B17), ISBLANK(C17)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B17, B$3-B17, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="17" t="str" cm="1">
-        <f t="array" ref="E18">_xlfn.IFS(OR(ISBLANK(B18), ISBLANK(C18)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B18, B$2-B18, TRUE, "N/A")</f>
+      <c r="A18" s="11"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="15" t="str" cm="1">
+        <f t="array" ref="E18">_xlfn.IFS(OR(ISBLANK(B18), ISBLANK(C18)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B18, B$3-B18, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="17" t="str" cm="1">
-        <f t="array" ref="E19">_xlfn.IFS(OR(ISBLANK(B19), ISBLANK(C19)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B19, B$2-B19, TRUE, "N/A")</f>
+      <c r="A19" s="11"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="15" t="str" cm="1">
+        <f t="array" ref="E19">_xlfn.IFS(OR(ISBLANK(B19), ISBLANK(C19)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B19, B$3-B19, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="17" t="str" cm="1">
-        <f t="array" ref="E20">_xlfn.IFS(OR(ISBLANK(B20), ISBLANK(C20)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B20, B$2-B20, TRUE, "N/A")</f>
+      <c r="A20" s="11"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="15" t="str" cm="1">
+        <f t="array" ref="E20">_xlfn.IFS(OR(ISBLANK(B20), ISBLANK(C20)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B20, B$3-B20, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="17" t="str" cm="1">
-        <f t="array" ref="E21">_xlfn.IFS(OR(ISBLANK(B21), ISBLANK(C21)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B21, B$2-B21, TRUE, "N/A")</f>
+      <c r="A21" s="11"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="15" t="str" cm="1">
+        <f t="array" ref="E21">_xlfn.IFS(OR(ISBLANK(B21), ISBLANK(C21)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B21, B$3-B21, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="17" t="str" cm="1">
-        <f t="array" ref="E22">_xlfn.IFS(OR(ISBLANK(B22), ISBLANK(C22)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B22, B$2-B22, TRUE, "N/A")</f>
+      <c r="A22" s="11"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="15" t="str" cm="1">
+        <f t="array" ref="E22">_xlfn.IFS(OR(ISBLANK(B22), ISBLANK(C22)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B22, B$3-B22, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="17" t="str" cm="1">
-        <f t="array" ref="E23">_xlfn.IFS(OR(ISBLANK(B23), ISBLANK(C23)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B23, B$2-B23, TRUE, "N/A")</f>
+      <c r="A23" s="11"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="15" t="str" cm="1">
+        <f t="array" ref="E23">_xlfn.IFS(OR(ISBLANK(B23), ISBLANK(C23)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B23, B$3-B23, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="17" t="str" cm="1">
-        <f t="array" ref="E24">_xlfn.IFS(OR(ISBLANK(B24), ISBLANK(C24)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B24, B$2-B24, TRUE, "N/A")</f>
+      <c r="A24" s="11"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="15" t="str" cm="1">
+        <f t="array" ref="E24">_xlfn.IFS(OR(ISBLANK(B24), ISBLANK(C24)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B24, B$3-B24, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="17" t="str" cm="1">
-        <f t="array" ref="E25">_xlfn.IFS(OR(ISBLANK(B25), ISBLANK(C25)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B25, B$2-B25, TRUE, "N/A")</f>
+      <c r="A25" s="11"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="15" t="str" cm="1">
+        <f t="array" ref="E25">_xlfn.IFS(OR(ISBLANK(B25), ISBLANK(C25)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B25, B$3-B25, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="17" t="str" cm="1">
-        <f t="array" ref="E26">_xlfn.IFS(OR(ISBLANK(B26), ISBLANK(C26)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B26, B$2-B26, TRUE, "N/A")</f>
+      <c r="A26" s="11"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="15" t="str" cm="1">
+        <f t="array" ref="E26">_xlfn.IFS(OR(ISBLANK(B26), ISBLANK(C26)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B26, B$3-B26, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="17" t="str" cm="1">
-        <f t="array" ref="E27">_xlfn.IFS(OR(ISBLANK(B27), ISBLANK(C27)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B27, B$2-B27, TRUE, "N/A")</f>
+      <c r="A27" s="11"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="15" t="str" cm="1">
+        <f t="array" ref="E27">_xlfn.IFS(OR(ISBLANK(B27), ISBLANK(C27)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B27, B$3-B27, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="17" t="str" cm="1">
-        <f t="array" ref="E28">_xlfn.IFS(OR(ISBLANK(B28), ISBLANK(C28)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B28, B$2-B28, TRUE, "N/A")</f>
+      <c r="A28" s="11"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="15" t="str" cm="1">
+        <f t="array" ref="E28">_xlfn.IFS(OR(ISBLANK(B28), ISBLANK(C28)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B28, B$3-B28, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="17" t="str" cm="1">
-        <f t="array" ref="E29">_xlfn.IFS(OR(ISBLANK(B29), ISBLANK(C29)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B29, B$2-B29, TRUE, "N/A")</f>
+      <c r="A29" s="11"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="15" t="str" cm="1">
+        <f t="array" ref="E29">_xlfn.IFS(OR(ISBLANK(B29), ISBLANK(C29)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B29, B$3-B29, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="17" t="str" cm="1">
-        <f t="array" ref="E30">_xlfn.IFS(OR(ISBLANK(B30), ISBLANK(C30)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B30, B$2-B30, TRUE, "N/A")</f>
+      <c r="A30" s="11"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="15" t="str" cm="1">
+        <f t="array" ref="E30">_xlfn.IFS(OR(ISBLANK(B30), ISBLANK(C30)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B30, B$3-B30, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="17" t="str" cm="1">
-        <f t="array" ref="E31">_xlfn.IFS(OR(ISBLANK(B31), ISBLANK(C31)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B31, B$2-B31, TRUE, "N/A")</f>
+      <c r="A31" s="11"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="15" t="str" cm="1">
+        <f t="array" ref="E31">_xlfn.IFS(OR(ISBLANK(B31), ISBLANK(C31)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B31, B$3-B31, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="17" t="str" cm="1">
-        <f t="array" ref="E32">_xlfn.IFS(OR(ISBLANK(B32), ISBLANK(C32)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B32, B$2-B32, TRUE, "N/A")</f>
+      <c r="A32" s="11"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="15" t="str" cm="1">
+        <f t="array" ref="E32">_xlfn.IFS(OR(ISBLANK(B32), ISBLANK(C32)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B32, B$3-B32, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="17" t="str" cm="1">
-        <f t="array" ref="E33">_xlfn.IFS(OR(ISBLANK(B33), ISBLANK(C33)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B33, B$2-B33, TRUE, "N/A")</f>
+      <c r="A33" s="11"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="15" t="str" cm="1">
+        <f t="array" ref="E33">_xlfn.IFS(OR(ISBLANK(B33), ISBLANK(C33)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B33, B$3-B33, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="17" t="str" cm="1">
-        <f t="array" ref="E34">_xlfn.IFS(OR(ISBLANK(B34), ISBLANK(C34)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B34, B$2-B34, TRUE, "N/A")</f>
+      <c r="A34" s="11"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="15" t="str" cm="1">
+        <f t="array" ref="E34">_xlfn.IFS(OR(ISBLANK(B34), ISBLANK(C34)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B34, B$3-B34, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="17" t="str" cm="1">
-        <f t="array" ref="E35">_xlfn.IFS(OR(ISBLANK(B35), ISBLANK(C35)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B35, B$2-B35, TRUE, "N/A")</f>
+      <c r="A35" s="11"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="15" t="str" cm="1">
+        <f t="array" ref="E35">_xlfn.IFS(OR(ISBLANK(B35), ISBLANK(C35)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B35, B$3-B35, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="17" t="str" cm="1">
-        <f t="array" ref="E36">_xlfn.IFS(OR(ISBLANK(B36), ISBLANK(C36)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B36, B$2-B36, TRUE, "N/A")</f>
+      <c r="A36" s="11"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="15" t="str" cm="1">
+        <f t="array" ref="E36">_xlfn.IFS(OR(ISBLANK(B36), ISBLANK(C36)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B36, B$3-B36, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="17" t="str" cm="1">
-        <f t="array" ref="E37">_xlfn.IFS(OR(ISBLANK(B37), ISBLANK(C37)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B37, B$2-B37, TRUE, "N/A")</f>
+      <c r="A37" s="11"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="15" t="str" cm="1">
+        <f t="array" ref="E37">_xlfn.IFS(OR(ISBLANK(B37), ISBLANK(C37)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B37, B$3-B37, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="17" t="str" cm="1">
-        <f t="array" ref="E38">_xlfn.IFS(OR(ISBLANK(B38), ISBLANK(C38)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B38, B$2-B38, TRUE, "N/A")</f>
+      <c r="A38" s="11"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="15" t="str" cm="1">
+        <f t="array" ref="E38">_xlfn.IFS(OR(ISBLANK(B38), ISBLANK(C38)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B38, B$3-B38, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="17" t="str" cm="1">
-        <f t="array" ref="E39">_xlfn.IFS(OR(ISBLANK(B39), ISBLANK(C39)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B39, B$2-B39, TRUE, "N/A")</f>
+      <c r="A39" s="11"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="15" t="str" cm="1">
+        <f t="array" ref="E39">_xlfn.IFS(OR(ISBLANK(B39), ISBLANK(C39)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B39, B$3-B39, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="17" t="str" cm="1">
-        <f t="array" ref="E40">_xlfn.IFS(OR(ISBLANK(B40), ISBLANK(C40)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B40, B$2-B40, TRUE, "N/A")</f>
+      <c r="A40" s="11"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="15" t="str" cm="1">
+        <f t="array" ref="E40">_xlfn.IFS(OR(ISBLANK(B40), ISBLANK(C40)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B40, B$3-B40, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="17" t="str" cm="1">
-        <f t="array" ref="E41">_xlfn.IFS(OR(ISBLANK(B41), ISBLANK(C41)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B41, B$2-B41, TRUE, "N/A")</f>
+      <c r="A41" s="11"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="15" t="str" cm="1">
+        <f t="array" ref="E41">_xlfn.IFS(OR(ISBLANK(B41), ISBLANK(C41)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B41, B$3-B41, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="17" t="str" cm="1">
-        <f t="array" ref="E42">_xlfn.IFS(OR(ISBLANK(B42), ISBLANK(C42)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B42, B$2-B42, TRUE, "N/A")</f>
+      <c r="A42" s="11"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="15" t="str" cm="1">
+        <f t="array" ref="E42">_xlfn.IFS(OR(ISBLANK(B42), ISBLANK(C42)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B42, B$3-B42, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="17" t="str" cm="1">
-        <f t="array" ref="E43">_xlfn.IFS(OR(ISBLANK(B43), ISBLANK(C43)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B43, B$2-B43, TRUE, "N/A")</f>
+      <c r="A43" s="11"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="15" t="str" cm="1">
+        <f t="array" ref="E43">_xlfn.IFS(OR(ISBLANK(B43), ISBLANK(C43)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B43, B$3-B43, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="17" t="str" cm="1">
-        <f t="array" ref="E44">_xlfn.IFS(OR(ISBLANK(B44), ISBLANK(C44)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B44, B$2-B44, TRUE, "N/A")</f>
+      <c r="A44" s="11"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="15" t="str" cm="1">
+        <f t="array" ref="E44">_xlfn.IFS(OR(ISBLANK(B44), ISBLANK(C44)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B44, B$3-B44, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="17" t="str" cm="1">
-        <f t="array" ref="E45">_xlfn.IFS(OR(ISBLANK(B45), ISBLANK(C45)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B45, B$2-B45, TRUE, "N/A")</f>
+      <c r="A45" s="11"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="15" t="str" cm="1">
+        <f t="array" ref="E45">_xlfn.IFS(OR(ISBLANK(B45), ISBLANK(C45)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B45, B$3-B45, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="17" t="str" cm="1">
-        <f t="array" ref="E46">_xlfn.IFS(OR(ISBLANK(B46), ISBLANK(C46)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B46, B$2-B46, TRUE, "N/A")</f>
+      <c r="A46" s="11"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="15" t="str" cm="1">
+        <f t="array" ref="E46">_xlfn.IFS(OR(ISBLANK(B46), ISBLANK(C46)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B46, B$3-B46, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="17" t="str" cm="1">
-        <f t="array" ref="E47">_xlfn.IFS(OR(ISBLANK(B47), ISBLANK(C47)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B47, B$2-B47, TRUE, "N/A")</f>
+      <c r="A47" s="11"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="15" t="str" cm="1">
+        <f t="array" ref="E47">_xlfn.IFS(OR(ISBLANK(B47), ISBLANK(C47)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B47, B$3-B47, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="17" t="str" cm="1">
-        <f t="array" ref="E48">_xlfn.IFS(OR(ISBLANK(B48), ISBLANK(C48)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B48, B$2-B48, TRUE, "N/A")</f>
+      <c r="A48" s="11"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="15" t="str" cm="1">
+        <f t="array" ref="E48">_xlfn.IFS(OR(ISBLANK(B48), ISBLANK(C48)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B48, B$3-B48, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="17" t="str" cm="1">
-        <f t="array" ref="E49">_xlfn.IFS(OR(ISBLANK(B49), ISBLANK(C49)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B49, B$2-B49, TRUE, "N/A")</f>
+      <c r="A49" s="11"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="15" t="str" cm="1">
+        <f t="array" ref="E49">_xlfn.IFS(OR(ISBLANK(B49), ISBLANK(C49)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B49, B$3-B49, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="17" t="str" cm="1">
-        <f t="array" ref="E50">_xlfn.IFS(OR(ISBLANK(B50), ISBLANK(C50)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B50, B$2-B50, TRUE, "N/A")</f>
+      <c r="A50" s="11"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="15" t="str" cm="1">
+        <f t="array" ref="E50">_xlfn.IFS(OR(ISBLANK(B50), ISBLANK(C50)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B50, B$3-B50, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="17" t="str" cm="1">
-        <f t="array" ref="E51">_xlfn.IFS(OR(ISBLANK(B51), ISBLANK(C51)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B51, B$2-B51, TRUE, "N/A")</f>
+      <c r="A51" s="11"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="15" t="str" cm="1">
+        <f t="array" ref="E51">_xlfn.IFS(OR(ISBLANK(B51), ISBLANK(C51)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B51, B$3-B51, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="15"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="17" t="str" cm="1">
-        <f t="array" ref="E52">_xlfn.IFS(OR(ISBLANK(B52), ISBLANK(C52)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B52, B$2-B52, TRUE, "N/A")</f>
+      <c r="A52" s="11"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="15" t="str" cm="1">
+        <f t="array" ref="E52">_xlfn.IFS(OR(ISBLANK(B52), ISBLANK(C52)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B52, B$3-B52, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="17" t="str" cm="1">
-        <f t="array" ref="E53">_xlfn.IFS(OR(ISBLANK(B53), ISBLANK(C53)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B53, B$2-B53, TRUE, "N/A")</f>
+      <c r="A53" s="11"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="15" t="str" cm="1">
+        <f t="array" ref="E53">_xlfn.IFS(OR(ISBLANK(B53), ISBLANK(C53)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B53, B$3-B53, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="17" t="str" cm="1">
-        <f t="array" ref="E54">_xlfn.IFS(OR(ISBLANK(B54), ISBLANK(C54)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$2&gt;B54, B$2-B54, TRUE, "N/A")</f>
+      <c r="A54" s="11"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="15" t="str" cm="1">
+        <f t="array" ref="E54">_xlfn.IFS(OR(ISBLANK(B54), ISBLANK(C54)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B54, B$3-B54, TRUE, "N/A")</f>
         <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="18"/>
+      <c r="A55" s="11"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="15" t="str" cm="1">
+        <f t="array" ref="E55">_xlfn.IFS(OR(ISBLANK(B55), ISBLANK(C55)), "Enter Data in 'Date of Expense' &amp; 'USD' as Needed", B$3&gt;B55, B$3-B55, TRUE, "N/A")</f>
+        <v>Enter Data in 'Date of Expense' &amp; 'USD' as Needed</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="15"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="18"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="16"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
-      <c r="B57" s="15"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="18"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="16"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="15"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="18"/>
+      <c r="A58" s="11"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="16"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="11"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B1:C1">
+  <conditionalFormatting sqref="B1:C1 B2">
     <cfRule type="containsBlanks" dxfId="7" priority="1">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>

</xml_diff>